<commit_message>
Fix issues with leading zero in CalEPA_CES data file
</commit_message>
<xml_diff>
--- a/output/geocoded.xlsx
+++ b/output/geocoded.xlsx
@@ -751,22 +751,22 @@
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>0.029592333</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>8.69794377</t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>70.5995828962491</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>18.5</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr"/>

</xml_diff>

<commit_message>
Add support for calculations involving values from data files
</commit_message>
<xml_diff>
--- a/output/geocoded.xlsx
+++ b/output/geocoded.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,175 +441,10 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>social_vulnerability_index</t>
+          <t>food_fraction_of_population_with_low_access</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>gini_inequality_coefficient</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>old_age_dependency_ratio</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>child_dependency_ratio</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>housing_median_year_built</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>housing_percent_occupied_units_lacking_plumbing</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>housing_percent_occupied_lacking_complete_kitchen</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>housing_percent_occupied_units_with_no_bedroom</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>housing_percent_occupied_units_with_no_vehicle_available</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>housing_percent_occupied_units_with_no_computer_included_smartphone</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>housing_percent_occupied_units_with_no_internet_subscription</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>population_density</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>percent_hispanic</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>percent_non_hispanic</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>percent_american_indian_or_alaska_native</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>percent_asian</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>percent_black</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>percent_native_hawaiian_or_other_pacific_islander</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>percent_multiple_race</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>percent_white</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>percent_some_other_race</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>percent_below_100_of_fed_poverty_level</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>percent_below_200_of_fed_poverty_level</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>percent_below_300_of_fed_poverty_level</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>percent_households_that_receive_snap</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>percent_households_with_limited_english</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>percent_bachelors_degree_age_25_or_over</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>median_household_income</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>unemployment_rate_age_16_or_over</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>air_quality_indicator_ozone_o3</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>air_quality_indicator_pm25</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>drinking_water_quality_indicator</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>air_quality_indicator_asthma_er_visits</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>food_fraction_of_population_with_low_access</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>food_low_access_tract</t>
         </is>
@@ -626,151 +461,10 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.0249</t>
+          <t>0.603631</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>0.4981</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>43.9</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>25.7</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1993</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2.2</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>25.7</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>96.7</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>19.2</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>4.1</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>5.4</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>68.1</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>3.6</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>789</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>200893</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>3.4</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>0.029592333</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>8.69794377</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>70.5995828962491</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>18.5</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr">
         <is>
           <t>1</t>
         </is>

</xml_diff>

<commit_message>
Implement Geocoding (using Census Geocoder)
</commit_message>
<xml_diff>
--- a/output/geocoded.xlsx
+++ b/output/geocoded.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,190 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>street</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>zip</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>SPATIAL_GEOID</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>social_vulnerability_index</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>gini_inequality_coefficient</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>old_age_dependency_ratio</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>child_dependency_ratio</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>housing_median_year_built</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>housing_percent_occupied_units_lacking_plumbing</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>housing_percent_occupied_lacking_complete_kitchen</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>housing_percent_occupied_units_with_no_bedroom</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>housing_percent_occupied_units_with_no_vehicle_available</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>housing_percent_occupied_units_with_no_computer_included_smartphone</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>housing_percent_occupied_units_with_no_internet_subscription</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>population_density</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>percent_hispanic</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>percent_non_hispanic</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>percent_american_indian_or_alaska_native</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>percent_asian</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>percent_black</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>percent_native_hawaiian_or_other_pacific_islander</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>percent_multiple_race</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>percent_white</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>percent_some_other_race</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>percent_below_100_of_fed_poverty_level</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>percent_households_that_receive_snap</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>percent_households_with_limited_english</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>percent_bachelors_degree_age_25_or_over</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>median_household_income</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>unemployment_rate_age_16_or_over</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>air_quality_indicator_ozone_o3</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>air_quality_indicator_pm25</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>drinking_water_quality_indicator</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>air_quality_indicator_asthma_er_visits</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>food_fraction_of_population_with_low_access</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>food_low_access_tract</t>
         </is>
@@ -456,17 +631,184 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>06001400100</t>
+          <t>1745 T Street Southeast</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.603631</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>20020</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>11001007605</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.5317</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>28.1</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1957</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>5.1</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>45.4</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>14.7</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>28.1</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>6.9</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>93.1</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>84.7</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>2.3</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>5.6</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>28.8</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>36.6</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>34.2</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>292</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>40239</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>10.3</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>Missing</t>
         </is>
       </c>
     </row>

</xml_diff>